<commit_message>
updating ipynb file for data cleansing and all output csv files
</commit_message>
<xml_diff>
--- a/Resources/CPI_ECI_Datasets/cpi-u_2013.xlsx
+++ b/Resources/CPI_ECI_Datasets/cpi-u_2013.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,26 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belindaho/Desktop/Analysis_Projects/Portfolio_Project/Portfolio_Project/Resources/CPI_ECI_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8275701-5625-4445-9474-9E5D5BDFB146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B6AAE-E3E7-1A49-9E9E-E906B9989E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="2" r:id="rId1"/>
     <sheet name="Regional" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1838,11 +1827,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="#0.0"/>
-    <numFmt numFmtId="166" formatCode="#0.00"/>
-    <numFmt numFmtId="167" formatCode="#0.000"/>
+    <numFmt numFmtId="164" formatCode="#0.0"/>
+    <numFmt numFmtId="165" formatCode="#0.00"/>
+    <numFmt numFmtId="166" formatCode="#0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1911,13 +1900,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="8"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2206,11 +2195,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR425"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="B361" sqref="B361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -56251,6 +56240,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="B421:AR421"/>
+    <mergeCell ref="B422:AR422"/>
+    <mergeCell ref="B423:AR423"/>
+    <mergeCell ref="B424:AR424"/>
+    <mergeCell ref="B425:AR425"/>
+    <mergeCell ref="B420:AR420"/>
+    <mergeCell ref="B409:AR409"/>
+    <mergeCell ref="B410:AR410"/>
+    <mergeCell ref="B411:AR411"/>
+    <mergeCell ref="B412:AR412"/>
+    <mergeCell ref="B413:AR413"/>
+    <mergeCell ref="B414:AR414"/>
+    <mergeCell ref="B415:AR415"/>
+    <mergeCell ref="B416:AR416"/>
+    <mergeCell ref="B417:AR417"/>
+    <mergeCell ref="B418:AR418"/>
+    <mergeCell ref="B419:AR419"/>
+    <mergeCell ref="B408:AR408"/>
+    <mergeCell ref="AJ5:AJ6"/>
+    <mergeCell ref="AK5:AK6"/>
+    <mergeCell ref="AL5:AL6"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="B7:AR7"/>
+    <mergeCell ref="B405:AR405"/>
+    <mergeCell ref="B406:AR406"/>
+    <mergeCell ref="B407:AR407"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AO5:AO6"/>
+    <mergeCell ref="AP5:AP6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AI6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="B1:AR1"/>
     <mergeCell ref="B2:AR2"/>
     <mergeCell ref="B3:AR3"/>
@@ -56267,63 +56313,6 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AO5:AO6"/>
-    <mergeCell ref="AP5:AP6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AI5:AI6"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="B7:AR7"/>
-    <mergeCell ref="B405:AR405"/>
-    <mergeCell ref="B406:AR406"/>
-    <mergeCell ref="B407:AR407"/>
-    <mergeCell ref="B408:AR408"/>
-    <mergeCell ref="AJ5:AJ6"/>
-    <mergeCell ref="AK5:AK6"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="B420:AR420"/>
-    <mergeCell ref="B409:AR409"/>
-    <mergeCell ref="B410:AR410"/>
-    <mergeCell ref="B411:AR411"/>
-    <mergeCell ref="B412:AR412"/>
-    <mergeCell ref="B413:AR413"/>
-    <mergeCell ref="B414:AR414"/>
-    <mergeCell ref="B421:AR421"/>
-    <mergeCell ref="B422:AR422"/>
-    <mergeCell ref="B423:AR423"/>
-    <mergeCell ref="B424:AR424"/>
-    <mergeCell ref="B425:AR425"/>
-    <mergeCell ref="B415:AR415"/>
-    <mergeCell ref="B416:AR416"/>
-    <mergeCell ref="B417:AR417"/>
-    <mergeCell ref="B418:AR418"/>
-    <mergeCell ref="B419:AR419"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
@@ -56332,10 +56321,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -59151,6 +59142,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B58:W58"/>
+    <mergeCell ref="B59:W59"/>
+    <mergeCell ref="B60:W60"/>
+    <mergeCell ref="B61:W61"/>
+    <mergeCell ref="B62:W62"/>
     <mergeCell ref="B57:W57"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -59161,11 +59157,6 @@
     <mergeCell ref="D4:Q4"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="U4:W4"/>
-    <mergeCell ref="B58:W58"/>
-    <mergeCell ref="B59:W59"/>
-    <mergeCell ref="B60:W60"/>
-    <mergeCell ref="B61:W61"/>
-    <mergeCell ref="B62:W62"/>
     <mergeCell ref="B6:W6"/>
     <mergeCell ref="B53:W53"/>
     <mergeCell ref="B54:W54"/>

</xml_diff>

<commit_message>
updated ipynb notebook, Tableau viz, and output files
</commit_message>
<xml_diff>
--- a/Resources/CPI_ECI_Datasets/cpi-u_2013.xlsx
+++ b/Resources/CPI_ECI_Datasets/cpi-u_2013.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belindaho/Desktop/Analysis_Projects/Portfolio_Project/Portfolio_Project/Resources/CPI_ECI_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B6AAE-E3E7-1A49-9E9E-E906B9989E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCE2C52-102E-B346-B57B-9EAE39925973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="2" r:id="rId1"/>
@@ -1833,10 +1833,15 @@
     <numFmt numFmtId="165" formatCode="#0.00"/>
     <numFmt numFmtId="166" formatCode="#0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1859,7 +1864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1915,6 +1920,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2198,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR425"/>
   <sheetViews>
-    <sheetView topLeftCell="A303" workbookViewId="0">
-      <selection activeCell="B361" sqref="B361"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B406" sqref="B406:AR406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -55242,7 +55250,7 @@
       <c r="A406" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B406" s="17" t="s">
+      <c r="B406" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C406" s="18"/>
@@ -56240,23 +56248,46 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B421:AR421"/>
-    <mergeCell ref="B422:AR422"/>
-    <mergeCell ref="B423:AR423"/>
-    <mergeCell ref="B424:AR424"/>
-    <mergeCell ref="B425:AR425"/>
-    <mergeCell ref="B420:AR420"/>
-    <mergeCell ref="B409:AR409"/>
-    <mergeCell ref="B410:AR410"/>
-    <mergeCell ref="B411:AR411"/>
-    <mergeCell ref="B412:AR412"/>
-    <mergeCell ref="B413:AR413"/>
-    <mergeCell ref="B414:AR414"/>
-    <mergeCell ref="B415:AR415"/>
-    <mergeCell ref="B416:AR416"/>
-    <mergeCell ref="B417:AR417"/>
-    <mergeCell ref="B418:AR418"/>
-    <mergeCell ref="B419:AR419"/>
+    <mergeCell ref="B1:AR1"/>
+    <mergeCell ref="B2:AR2"/>
+    <mergeCell ref="B3:AR3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:P4"/>
+    <mergeCell ref="Q4:AC4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AN4"/>
+    <mergeCell ref="AO4:AR4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AI6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
     <mergeCell ref="B408:AR408"/>
     <mergeCell ref="AJ5:AJ6"/>
     <mergeCell ref="AK5:AK6"/>
@@ -56273,46 +56304,23 @@
     <mergeCell ref="AP5:AP6"/>
     <mergeCell ref="AD5:AD6"/>
     <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AI5:AI6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="B1:AR1"/>
-    <mergeCell ref="B2:AR2"/>
-    <mergeCell ref="B3:AR3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:P4"/>
-    <mergeCell ref="Q4:AC4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AN4"/>
-    <mergeCell ref="AO4:AR4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B420:AR420"/>
+    <mergeCell ref="B409:AR409"/>
+    <mergeCell ref="B410:AR410"/>
+    <mergeCell ref="B411:AR411"/>
+    <mergeCell ref="B412:AR412"/>
+    <mergeCell ref="B413:AR413"/>
+    <mergeCell ref="B414:AR414"/>
+    <mergeCell ref="B415:AR415"/>
+    <mergeCell ref="B416:AR416"/>
+    <mergeCell ref="B417:AR417"/>
+    <mergeCell ref="B418:AR418"/>
+    <mergeCell ref="B419:AR419"/>
+    <mergeCell ref="B421:AR421"/>
+    <mergeCell ref="B422:AR422"/>
+    <mergeCell ref="B423:AR423"/>
+    <mergeCell ref="B424:AR424"/>
+    <mergeCell ref="B425:AR425"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
@@ -56324,8 +56332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -59142,11 +59150,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B58:W58"/>
-    <mergeCell ref="B59:W59"/>
-    <mergeCell ref="B60:W60"/>
-    <mergeCell ref="B61:W61"/>
-    <mergeCell ref="B62:W62"/>
     <mergeCell ref="B57:W57"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
@@ -59162,6 +59165,11 @@
     <mergeCell ref="B54:W54"/>
     <mergeCell ref="B55:W55"/>
     <mergeCell ref="B56:W56"/>
+    <mergeCell ref="B58:W58"/>
+    <mergeCell ref="B59:W59"/>
+    <mergeCell ref="B60:W60"/>
+    <mergeCell ref="B61:W61"/>
+    <mergeCell ref="B62:W62"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>

</xml_diff>